<commit_message>
Recommit all the Files.
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/TestCaseData.xlsx
+++ b/SeleniumAutomationFramework/src/TestCaseData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,66 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>zTestFirstName</t>
+  </si>
+  <si>
+    <t>zTestMiddleName</t>
+  </si>
+  <si>
+    <t>zTestLastName</t>
+  </si>
+  <si>
+    <t>Fifth grade</t>
+  </si>
+  <si>
+    <t>prefname</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Suffix</t>
+  </si>
+  <si>
+    <t>Preferred Name</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -47,13 +101,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -388,13 +446,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
+    <col min="2" max="2" width="24.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -407,10 +519,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Committing the code to do the merge.
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/TestCaseData.xlsx
+++ b/SeleniumAutomationFramework/src/TestCaseData.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="1" r:id="rId1"/>
-    <sheet name="Class" sheetId="2" r:id="rId2"/>
+    <sheet name="Add Class" sheetId="2" r:id="rId2"/>
+    <sheet name="Edit Class" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,22 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>zTestFirstName</t>
-  </si>
-  <si>
-    <t>zTestMiddleName</t>
-  </si>
-  <si>
-    <t>zTestLastName</t>
-  </si>
-  <si>
-    <t>Fifth grade</t>
-  </si>
-  <si>
-    <t>prefname</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>First Name</t>
   </si>
@@ -52,14 +38,119 @@
     <t>Suffix</t>
   </si>
   <si>
-    <t>Preferred Name</t>
+    <t>display_name</t>
+  </si>
+  <si>
+    <t>Kleimo</t>
+  </si>
+  <si>
+    <t>Ms</t>
+  </si>
+  <si>
+    <t>Ally</t>
+  </si>
+  <si>
+    <t>Chandy</t>
+  </si>
+  <si>
+    <t>Kathleen</t>
+  </si>
+  <si>
+    <t>Gary</t>
+  </si>
+  <si>
+    <t>Sabreen</t>
+  </si>
+  <si>
+    <t>Jonah</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Somnam</t>
+  </si>
+  <si>
+    <t>Wendy</t>
+  </si>
+  <si>
+    <t>Windy</t>
+  </si>
+  <si>
+    <t>Gina</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Wen</t>
+  </si>
+  <si>
+    <t>Kelly Leitz</t>
+  </si>
+  <si>
+    <t>Esmeralda</t>
+  </si>
+  <si>
+    <t>Higgenbotham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamie </t>
+  </si>
+  <si>
+    <t>Jessie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esmeralda </t>
+  </si>
+  <si>
+    <t>Kelsch</t>
+  </si>
+  <si>
+    <t>Hydrick</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Karina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carlene </t>
+  </si>
+  <si>
+    <t>Dorfman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kelly </t>
+  </si>
+  <si>
+    <t>Ellzey</t>
+  </si>
+  <si>
+    <t>Veney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benita </t>
+  </si>
+  <si>
+    <t>Ribas</t>
+  </si>
+  <si>
+    <t>Bellman</t>
+  </si>
+  <si>
+    <t>Eaglin</t>
+  </si>
+  <si>
+    <t>First grade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,6 +173,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,8 +203,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -446,67 +545,249 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.625" customWidth="1"/>
-    <col min="2" max="2" width="24.75" customWidth="1"/>
+    <col min="2" max="2" width="47.25" customWidth="1"/>
+    <col min="4" max="4" width="14.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="B1" t="str">
+        <f ca="1">INDEX(C1:C24,INT(RAND()*24+1))</f>
+        <v>Gina</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f ca="1">INDEX(D1:D24,INT(RAND()*24+1))</f>
+        <v>Ribas</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -517,17 +798,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="16" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f ca="1">CONCATENATE("Class", RAND())</f>
+        <v>Class0.022760801371992</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="str">
+        <f ca="1">'Add Class'!B1</f>
+        <v>Class0.022760801371992</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>